<commit_message>
Added Supply Minimum field. If actual Supply Quantity is less than Supply Minimum then item will be posted.
</commit_message>
<xml_diff>
--- a/Homeless Mission Supply List.xlsx
+++ b/Homeless Mission Supply List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffouquet\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Documents\UiPath\NPOProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D81897-0BCE-4E0E-885C-8DF1FBA1E963}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DE8352-5802-4E89-B012-D8708E396CE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="8" xr2:uid="{D50DBB5C-06FE-47F5-85D1-E1104E8C8C5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{D50DBB5C-06FE-47F5-85D1-E1104E8C8C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Eggs &amp; Dairy" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Fruits and Vegetables" sheetId="5" r:id="rId3"/>
     <sheet name="Meat" sheetId="6" r:id="rId4"/>
     <sheet name="Pantry" sheetId="1" r:id="rId5"/>
-    <sheet name="Bevereges" sheetId="4" r:id="rId6"/>
-    <sheet name="Hygeine &amp; Personal Care" sheetId="7" r:id="rId7"/>
+    <sheet name="Beverages" sheetId="4" r:id="rId6"/>
+    <sheet name="Hygene &amp; Personal Care" sheetId="7" r:id="rId7"/>
     <sheet name="Household Essentials" sheetId="2" r:id="rId8"/>
     <sheet name=" Baby &amp; Childcare" sheetId="9" r:id="rId9"/>
   </sheets>
@@ -3254,7 +3254,7 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3563,7 +3563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500975C-61A2-4D63-932D-349F4E4BED3D}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>